<commit_message>
figures for pilot data and modified nback frame duration
</commit_message>
<xml_diff>
--- a/Checking performance and rt graphs.xlsx
+++ b/Checking performance and rt graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocel\Documents\Collab project Marco Pang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joce\Documents\Jocelyn\PolyU RA\collab-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3327BB93-4EA5-4CB1-9074-2912AFE94AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA253CAE-1DF0-4A0A-B79A-1334663409CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Stroop</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Average reaction time and performance per task across all participants</t>
+  </si>
+  <si>
+    <t>Stroop performance by condition</t>
+  </si>
+  <si>
+    <t>Stroop reaction time by condition</t>
+  </si>
+  <si>
+    <t>Congruent</t>
+  </si>
+  <si>
+    <t>Incongruent</t>
+  </si>
+  <si>
+    <t>Neutral</t>
   </si>
 </sst>
 </file>
@@ -368,13 +383,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>488948</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -429,13 +444,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>555625</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -490,13 +505,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -551,13 +566,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -590,6 +605,250 @@
         <a:xfrm>
           <a:off x="14630400" y="4762499"/>
           <a:ext cx="4889500" cy="3667125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C985D4A1-3062-A48D-A9ED-D4902908F8DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="4572000"/>
+          <a:ext cx="4800600" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F8A895C-497F-4E62-A293-694BDFED5F81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="12473940"/>
+          <a:ext cx="6858000" cy="4114800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34FE5829-4E2E-39AA-EF41-2E9685FAE655}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5730240" y="4572000"/>
+          <a:ext cx="4800600" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C5D401A-571C-E967-339F-8389264A7B53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11216640" y="4572000"/>
+          <a:ext cx="4800600" cy="2743200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -874,86 +1133,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096954AC-DA63-4380-A37D-1B9AEC94D1B7}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B94" t="s">
         <v>0</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C94" t="s">
         <v>1</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D94" t="s">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E94" t="s">
         <v>6</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F94" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>3</v>
       </c>
-      <c r="B49">
+      <c r="B95">
         <v>0.94752999999999998</v>
       </c>
-      <c r="C49">
+      <c r="C95">
         <v>0.82500000000000007</v>
       </c>
-      <c r="D49">
+      <c r="D95">
         <v>0.69166666666666676</v>
       </c>
-      <c r="E49">
+      <c r="E95">
         <v>0.71666666666666679</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>4</v>
       </c>
-      <c r="B50">
+      <c r="B96">
         <v>0.90433320133378958</v>
       </c>
-      <c r="C50">
+      <c r="C96">
         <v>1.4835397411756868</v>
       </c>
-      <c r="D50">
+      <c r="D96">
         <v>0.96099349570133663</v>
       </c>
-      <c r="E50">
+      <c r="E96">
         <v>0.89863720718502504</v>
       </c>
-      <c r="F50">
+      <c r="F96">
         <v>1.2156666666666667</v>
       </c>
     </row>

</xml_diff>